<commit_message>
sua dinh dang ket qua, them icon
</commit_message>
<xml_diff>
--- a/getlocation/bin/Debug/EndSource.xlsx
+++ b/getlocation/bin/Debug/EndSource.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <x:si>
     <x:t>Dia Chi</x:t>
   </x:si>
@@ -22,58 +22,76 @@
     <x:t>Location</x:t>
   </x:si>
   <x:si>
-    <x:t>347/13 Chu Văn An, phường 11, Bình Thạnh</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10.812843,106.700371</x:t>
-  </x:si>
-  <x:si>
-    <x:t>373/33, Lý thường kiệt, phường 9, tân binh, tphcm,Hồ Chí Minh,Quận Tân Bình,Phường 9 , Quận Tân Bình</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10.780088,106.654209</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Số 52 ngõ 204 kim Giang, Phường Kim Giang, Quận Thanh Xuân, Hà Nội</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20.983920,105.811852</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Cali Tower, 464-466-468 Phan Xích Long, Phường 02, Quận Phú Nhuận, Hồ Chí Minh</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10.801453,106.683885</x:t>
-  </x:si>
-  <x:si>
-    <x:t>171 , võ văn ngân, Phường Linh Chiểu, Quận Thủ Đức, Hồ Chí Minh</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10.850800,106.763558</x:t>
-  </x:si>
-  <x:si>
-    <x:t>275/110 - Quang Trung - Phường 10 - Quận Gò Vấp,Hồ Chí Minh,Quận Gò Vấp,Phường 10 , Quận Gò Vấp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10.828067,106.670617</x:t>
-  </x:si>
-  <x:si>
-    <x:t>37 NGUYỄN BÁ TÒNG, P. TÂN THÀNH, Q. TÂN PHÚ. HCM, TÂN PHÚ, Hồ Chí Minh37 NGUYỄN BÁ TÒNG, P. TÂN THÀNH, Q. TÂN PHÚ. HCM Hồ Chí Minh, TÂN PHÚ , Quận Tân Phú</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10.801465,106.652597</x:t>
-  </x:si>
-  <x:si>
-    <x:t>312 Nguyễn Thượng Hiền Hồ Chí Minh, Quận Phú Nhuận, Phường 05 , Phường 05 , Quận Phú Nhuận , Hồ Chí Minh</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10.805653,106.685203</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Huyện Bình Chánh, Hồ Chí Minh, Xã An Phú Tây, c10/18 ql1a, , Huyện Bình Chánh</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10.683530,106.605409</x:t>
+    <x:t>758 nguyen binh, Hồ Chí Minh, Huyện Nhà Bè, Xã Nhơn Đức , Huyện Nhà Bè</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10.672910, 106.710321</x:t>
+  </x:si>
+  <x:si>
+    <x:t>137A Nguyễn Văn Cừ - Long Biên - Hà Nội, Phường Ngọc Lâm, Quận Long Biên, Hà Nội</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21.042771, 105.870831</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lữ Đoàn 45 , Cổ Đông , Sơn Tây, Hà nội, Hà Nội, Thành Phố Sơn Tây, Xã Cổ Đông , Thành Phố Sơn Tây</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21.04679, 105.505885</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Số 46 tổ 12, Phường Sài Đồng, Quận Long Biên, Hà Nội</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21.027864, 105.910237</x:t>
+  </x:si>
+  <x:si>
+    <x:t>số 8 ngõ 191 phạm văn đồng, Phường Xuân Đỉnh, Quận Bắc Từ Liêm, Hà Nội</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21.065679, 105.785899</x:t>
+  </x:si>
+  <x:si>
+    <x:t>60/1, Xã Bà Điểm, Huyện Hóc Môn, Hồ Chí Minh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10.864291, 106.564633</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cầu cảng số 12, đường hồ học lãm, p16, q8, tp.hcm, Phường 16, Quận 8, Hồ Chí Minh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10.710249, 106.613956</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Số 4 tổ 51 cụm 8 Phú thượng Tây Hồ ( Chân cầu Nhật Tân ), Phường Phú Thượng, Quận Tây Hồ, Hà Nội</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21.089703, 105.819309</x:t>
+  </x:si>
+  <x:si>
+    <x:t>so12 duong ht25 phuong hiep thanh q12.cty hoang vinh ha, Phường Hiệp Thành, Quận 12, Hồ Chí Minh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10.882629, 106.640076</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Số 17 vạn phúc, Phường Kim Mã, Quận Ba Đình, Hà Nội</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21.033091, 105.81955</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Số 16 phố viên, gần viện bảo vệ Thực vật, Phường Cổ Nhuế 2, Quận Bắc Từ Liêm, Hà Nội</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21.066698, 105.772828</x:t>
+  </x:si>
+  <x:si>
+    <x:t>68 Đường 1a Tổ3 kp Giản Dân phường Long Thạnh Mỹ Q9, Phường Long Thạnh Mỹ, Quận 9, Hồ Chí Minh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10.847253, 106.765632</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -137,8 +155,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B10" totalsRowShown="0">
-  <x:autoFilter ref="A1:B10"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B13" totalsRowShown="0">
+  <x:autoFilter ref="A1:B13"/>
   <x:tableColumns count="2">
     <x:tableColumn id="1" name="Dia Chi"/>
     <x:tableColumn id="2" name="Location"/>
@@ -435,14 +453,14 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B10"/>
+  <x:dimension ref="A1:B13"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="151.690625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="21.470625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="91.000625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="21.950625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:2">
@@ -523,6 +541,30 @@
       </x:c>
       <x:c r="B10" s="0" t="s">
         <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:2">
+      <x:c r="A11" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:2">
+      <x:c r="A12" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:2">
+      <x:c r="A13" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>25</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>